<commit_message>
Changed Mortality Assessment Data
</commit_message>
<xml_diff>
--- a/data/usda-families/mortality/20250513_mortality.xlsx
+++ b/data/usda-families/mortality/20250513_mortality.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolynkounellas/Documents/GitHub/resazurin-assay-development/data/usda-families/mortality/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolynkounellas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D666E5-DA97-4F44-BF49-5E773CE423BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1B1E6B-22DA-4F40-9BE9-6BBE34AB14E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="3560" windowWidth="28040" windowHeight="16900" xr2:uid="{F2EBC79F-879C-C244-AACF-32B6A2FCF28D}"/>
+    <workbookView xWindow="1880" yWindow="2480" windowWidth="28040" windowHeight="16900" xr2:uid="{F2EBC79F-879C-C244-AACF-32B6A2FCF28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Sample</t>
   </si>
@@ -117,15 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dead or Alive </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dead </t>
-  </si>
-  <si>
-    <t>Alive</t>
-  </si>
-  <si>
-    <t>Dead</t>
   </si>
 </sst>
 </file>
@@ -508,7 +499,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,200 +519,200 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
+      <c r="B2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
+      <c r="B3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
+      <c r="B8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
+      <c r="B9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
+      <c r="B10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
+      <c r="B11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
+      <c r="B12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
+      <c r="B13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
+      <c r="B14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
+      <c r="B15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
+      <c r="B16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
+      <c r="B17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
+      <c r="B18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>28</v>
+      <c r="B19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>28</v>
+      <c r="B20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>28</v>
+      <c r="B21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
+      <c r="B22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>28</v>
+      <c r="B23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>28</v>
+      <c r="B24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>28</v>
+      <c r="B25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>28</v>
+      <c r="B26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>